<commit_message>
Fix small bug, update data, get historical points on chart
</commit_message>
<xml_diff>
--- a/data/brasil.xlsx
+++ b/data/brasil.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Confronto_operações" sheetId="1" state="visible" r:id="rId3"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="140">
   <si>
     <t xml:space="preserve">yearmo</t>
   </si>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">2017m5</t>
   </si>
   <si>
-    <t xml:space="preserve">Marcha basta de violência 24.5.2017</t>
+    <t xml:space="preserve">Marcha basta de violência 2017m5</t>
   </si>
   <si>
     <t xml:space="preserve">2017m6</t>
@@ -190,7 +190,25 @@
     <t xml:space="preserve">2018m2</t>
   </si>
   <si>
-    <t xml:space="preserve">Intervenção federal começa 16.2.2023</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Intervenção federal começa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">2018m2</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">2018m3</t>
@@ -223,7 +241,7 @@
     <t xml:space="preserve">2018m12</t>
   </si>
   <si>
-    <t xml:space="preserve">intervenção federal termina 31.12/2023</t>
+    <t xml:space="preserve">intervenção federal termina 2018m12</t>
   </si>
   <si>
     <t xml:space="preserve">2019m1</t>
@@ -277,7 +295,7 @@
     <t xml:space="preserve">2020m5</t>
   </si>
   <si>
-    <t xml:space="preserve">ADPF - Maio 2020</t>
+    <t xml:space="preserve">ADPF 2020m5</t>
   </si>
   <si>
     <t xml:space="preserve">2020m6</t>
@@ -476,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -512,6 +530,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -614,19 +638,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -825,12 +849,12 @@
   </sheetPr>
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8166,12 +8190,12 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q7" activeCellId="0" sqref="Q7"/>
+      <selection pane="bottomRight" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8195,7 +8219,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="21.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="20" style="1" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="36.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="22" style="1" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8259,6 +8285,9 @@
       <c r="T1" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="U1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -8273,6 +8302,7 @@
       <c r="K2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -8555,6 +8585,7 @@
       <c r="T14" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="U14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
@@ -8802,6 +8833,9 @@
       </c>
       <c r="T18" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9305,6 +9339,7 @@
       <c r="T26" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="U26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
@@ -9367,6 +9402,9 @@
       <c r="T27" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="U27" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
@@ -9987,7 +10025,9 @@
       <c r="T37" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U37" s="4"/>
+      <c r="U37" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
@@ -11052,6 +11092,9 @@
       </c>
       <c r="T54" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>